<commit_message>
find the reason of 52 --- node 771&780 and related edges
</commit_message>
<xml_diff>
--- a/data/Metro 52 Noord = Zuid.xlsx
+++ b/data/Metro 52 Noord = Zuid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\UTNCE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432C5216-7D32-4AF9-AA3A-C06A8208C4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E9B4D9-18E8-4893-BCFC-65660B83D64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,53 +25,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Station Zuid</t>
   </si>
   <si>
-    <t>13:31 + 1</t>
-  </si>
-  <si>
-    <t>13:38 + 1</t>
-  </si>
-  <si>
     <t>Europaplein</t>
   </si>
   <si>
-    <t>13:33 + 1</t>
-  </si>
-  <si>
-    <t>13:41 + 1</t>
-  </si>
-  <si>
     <t>De Pijp</t>
   </si>
   <si>
-    <t>13:35 + 1</t>
-  </si>
-  <si>
-    <t>13:43 + 1</t>
-  </si>
-  <si>
     <t>Vijzelgracht</t>
   </si>
   <si>
-    <t>13:37 + 1</t>
-  </si>
-  <si>
-    <t>13:44 + 1</t>
-  </si>
-  <si>
     <t>Rokin</t>
   </si>
   <si>
-    <t>13:39 + 1</t>
-  </si>
-  <si>
-    <t>13:46 + 1</t>
-  </si>
-  <si>
     <t>Centraal Station</t>
   </si>
   <si>
@@ -79,9 +49,6 @@
   </si>
   <si>
     <t>Noord</t>
-  </si>
-  <si>
-    <t>13:45 + 1</t>
   </si>
 </sst>
 </file>
@@ -402,173 +369,174 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>0.7104166666666667</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3" s="1">
+        <v>0.71388888888888891</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.57361111111111118</v>
+        <v>0.71736111111111101</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6" s="1">
+        <v>0.71180555555555547</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
+      <c r="A7" s="1">
+        <v>0.71527777777777779</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.57500000000000007</v>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
+      <c r="A10" s="1">
+        <v>0.71319444444444446</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
+      <c r="A11" s="1">
+        <v>0.71666666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>0.57638888888888895</v>
+        <v>0.72013888888888899</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
+      <c r="A14" s="1">
+        <v>0.71458333333333324</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
+      <c r="A15" s="1">
+        <v>0.71805555555555556</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>0.57777777777777783</v>
+        <v>0.72152777777777777</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
+      <c r="A18" s="1">
+        <v>0.71597222222222223</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
+      <c r="A19" s="1">
+        <v>0.71944444444444444</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.57916666666666672</v>
+        <v>0.72291666666666676</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
+      <c r="A22" s="1">
+        <v>0.71736111111111101</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>0.57500000000000007</v>
+        <v>0.72083333333333333</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>0.5805555555555556</v>
+        <v>0.72430555555555554</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>8</v>
+      <c r="A26" s="1">
+        <v>0.71875</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>0.57638888888888895</v>
+        <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>0.58194444444444449</v>
+        <v>0.72569444444444453</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>18</v>
+      <c r="A30" s="1">
+        <v>0.72013888888888899</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>0.57847222222222217</v>
+        <v>0.72361111111111109</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>0.58333333333333337</v>
+        <v>0.7270833333333333</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>